<commit_message>
refactor: Clean up ContentPage component by reorganizing imports and removing unused code; enhance Excel generation utility with default values for readings and column width settings
</commit_message>
<xml_diff>
--- a/tmp/Readings.xlsx
+++ b/tmp/Readings.xlsx
@@ -397,10 +397,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" customWidth="1"/>
+    <col min="18" max="18" width="30.83203125" customWidth="1"/>
+    <col min="19" max="19" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -410,57 +431,54 @@
         <v>л/с №</v>
       </c>
       <c r="C1" t="str">
-        <v>телефон</v>
+        <v>ФИО</v>
       </c>
       <c r="D1" t="str">
-        <v>ФИО</v>
+        <v>Адрес</v>
       </c>
       <c r="E1" t="str">
-        <v>Адрес</v>
+        <v>(1)ХВС с/у</v>
       </c>
       <c r="F1" t="str">
-        <v>(1)ХВС с/у</v>
+        <v>(2)ГВС с/у</v>
       </c>
       <c r="G1" t="str">
-        <v>(2)ГВС с/у</v>
+        <v>(3)ХВС кух</v>
       </c>
       <c r="H1" t="str">
-        <v>(3)ХВС кух</v>
+        <v>(4)ГВС кух</v>
       </c>
       <c r="I1" t="str">
-        <v>(4)ГВС кух</v>
+        <v>(5)ХВС с/у</v>
       </c>
       <c r="J1" t="str">
-        <v>(5)ХВС с/у</v>
+        <v>(6)ГВС с/у</v>
       </c>
       <c r="K1" t="str">
-        <v>(6)ГВС с/у</v>
+        <v>Вд №</v>
       </c>
       <c r="L1" t="str">
-        <v>Вд №</v>
+        <v>(6)ХВС (скваж)</v>
       </c>
       <c r="M1" t="str">
-        <v>(6)ХВС (скваж)</v>
+        <v>(7)ХВС с/у(гр)</v>
       </c>
       <c r="N1" t="str">
-        <v>(7)ХВС с/у(гр)</v>
+        <v>(8)ХВС кух(гр)</v>
       </c>
       <c r="O1" t="str">
-        <v>(8)ХВС кух(гр)</v>
+        <v>(9)ГВС с/у(гр)</v>
       </c>
       <c r="P1" t="str">
-        <v>(9)ГВС с/у(гр)</v>
+        <v>(10)ГВС кух(гр)</v>
       </c>
       <c r="Q1" t="str">
-        <v>(10)ГВС кух(гр)</v>
+        <v>(11)ХВС туалет(гр)</v>
       </c>
       <c r="R1" t="str">
-        <v>(11)ХВС туалет(гр)</v>
+        <v>(12)ХВС ванна, титан(гр)</v>
       </c>
       <c r="S1" t="str">
-        <v>(12)ХВС ванна, титан(гр)</v>
-      </c>
-      <c r="T1" t="str">
         <v>(14)ГВС туалет(гр)</v>
       </c>
     </row>
@@ -469,37 +487,37 @@
         <v>25.07.2025</v>
       </c>
       <c r="B2" t="str">
-        <v>4123q4-13412-4124</v>
+        <v>55-45-2</v>
       </c>
       <c r="C2" t="str">
-        <v>+7</v>
+        <v>55</v>
       </c>
       <c r="D2" t="str">
-        <v>1234</v>
+        <v>Арес очень далекий как звезды</v>
       </c>
       <c r="E2" t="str">
-        <v>123412</v>
+        <v>442</v>
       </c>
       <c r="F2" t="str">
-        <v>341234</v>
+        <v>4431</v>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>552</v>
       </c>
       <c r="H2" t="str">
-        <v/>
+        <v>666</v>
       </c>
       <c r="I2" t="str">
-        <v/>
+        <v>6356</v>
       </c>
       <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <v/>
-      </c>
-      <c r="L2">
-        <v>0</v>
+        <v>266</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="str">
+        <v>6636</v>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -520,9 +538,6 @@
         <v/>
       </c>
       <c r="S2" t="str">
-        <v/>
-      </c>
-      <c r="T2" t="str">
         <v/>
       </c>
     </row>
@@ -531,40 +546,40 @@
         <v>25.07.2025</v>
       </c>
       <c r="B3" t="str">
-        <v>52345-2435-542345</v>
+        <v>52345-5423-54235</v>
       </c>
       <c r="C3" t="str">
-        <v>+7</v>
+        <v>5423</v>
       </c>
       <c r="D3" t="str">
-        <v>2345</v>
-      </c>
-      <c r="E3" t="str">
-        <v>234523</v>
-      </c>
-      <c r="F3" t="str">
-        <v>52345</v>
-      </c>
-      <c r="G3" t="str">
-        <v>52435</v>
-      </c>
-      <c r="H3" t="str">
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
+        <v>54235</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3" t="str">
-        <v/>
+      <c r="M3">
+        <v>0</v>
       </c>
       <c r="N3" t="str">
         <v/>
@@ -584,13 +599,128 @@
       <c r="S3" t="str">
         <v/>
       </c>
-      <c r="T3" t="str">
-        <v/>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>25.07.2025</v>
+      </c>
+      <c r="B4" t="str">
+        <v>52-34243-52345</v>
+      </c>
+      <c r="C4" t="str">
+        <v>23452345</v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v>2345235</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <v>2</v>
+      </c>
+      <c r="I4" t="str">
+        <v>4352435</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>25.07.2025</v>
+      </c>
+      <c r="B5" t="str">
+        <v>55--</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>